<commit_message>
rewrite filter search logic for new UI, add location options
</commit_message>
<xml_diff>
--- a/Company List.xlsx
+++ b/Company List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Samir/uc-berkeley/dss/dss-sourcing/Sourcing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tutrinh/Work/DSS/Sourcing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC066281-C1FB-9749-B98E-C8FBB7BDA4D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06E001D-58E3-784F-BB42-085852F5693A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="460" windowWidth="28040" windowHeight="16600" xr2:uid="{D83C6B3A-4F92-0D40-A388-143AAD2E14F7}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{D83C6B3A-4F92-0D40-A388-143AAD2E14F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>Amazon</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D472012-5252-4A4F-89F1-EF44BBB83C52}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -395,6 +398,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update README, clean up code, revert to template settings
</commit_message>
<xml_diff>
--- a/Company List.xlsx
+++ b/Company List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tutrinh/Work/DSS/Sourcing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06E001D-58E3-784F-BB42-085852F5693A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9D9797-5A2F-F94D-B378-78EA480ABE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{D83C6B3A-4F92-0D40-A388-143AAD2E14F7}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Company</t>
-  </si>
-  <si>
-    <t>Amazon</t>
   </si>
 </sst>
 </file>
@@ -382,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D472012-5252-4A4F-89F1-EF44BBB83C52}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -398,11 +395,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>